<commit_message>
Updated requirements to model, deleted Netlogo comment
- Updated requirements to what actually happens in the model.
- Deleted a comment about building damage coming later (already implemented)  in the actual model.
</commit_message>
<xml_diff>
--- a/conceptualisation/Requirements.xlsx
+++ b/conceptualisation/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\Github\SEN1211-earthquake-project\conceptualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CE9F5D-F38F-4D61-BD4D-689FB992F2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8C3A0E-2FB5-40AB-9E9D-7DB974166FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{574AE5E0-4647-4F58-AFB1-1899A91ECA14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{574AE5E0-4647-4F58-AFB1-1899A91ECA14}"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="102">
   <si>
     <t>Drone flying time is affected by movement and hovering</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>Only a single earthquake event at the start of the simulation</t>
-  </si>
-  <si>
-    <t>The earthquake has a certain magnitude drawn by a random distribution</t>
   </si>
   <si>
     <t>Building vulnerability depends on the building type (concrete/brick), building height, distance from epicenter multiplier and the earthquake intensity multiplier.</t>
@@ -224,9 +221,6 @@
     <t>The farthest building from the earthquake epicenter has a vulnerability of 0 due to the Building Vulnerability formula.</t>
   </si>
   <si>
-    <t>The earthquake can be created on any place inside or outside of the city.</t>
-  </si>
-  <si>
     <t>RE</t>
   </si>
   <si>
@@ -357,6 +351,33 @@
   </si>
   <si>
     <t>The amount of residents in each building depends on the height of the building and some random distribution</t>
+  </si>
+  <si>
+    <t>Ambulances dron't drive over roads in the model. They jump from crossing to crossing</t>
+  </si>
+  <si>
+    <t>The building type is determined by a random distribution which depends on a slider. The slider says how much percent of the buildings is from concrete.</t>
+  </si>
+  <si>
+    <t>The only possible values for building-type are 1 and 0.5.</t>
+  </si>
+  <si>
+    <t>The earthquake can be created on any place inside or outside of the city (but within model).</t>
+  </si>
+  <si>
+    <t>Hospitals have the color white and size 12.</t>
+  </si>
+  <si>
+    <t>When a crossing is chosen to be a hospital, the breed of the crossing changes to 'hospitals'.</t>
+  </si>
+  <si>
+    <t>The only possible values for building-height are 1 (tall), 0.6 (medium and 0.2 (small).</t>
+  </si>
+  <si>
+    <t>The patches in the epicenter of the earthquake are black, patches far from the earthquake are white. There is a gradient in between.</t>
+  </si>
+  <si>
+    <t>The earthquake has a certain magnitude determined by a slider.</t>
   </si>
 </sst>
 </file>
@@ -731,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA006879-D9B2-4595-ABCF-2B2B08F25C3A}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,10 +770,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -763,10 +784,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -777,10 +798,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -791,94 +812,94 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12">
         <v>6</v>
@@ -889,10 +910,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13">
         <v>7</v>
@@ -903,10 +924,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14">
         <v>8</v>
@@ -917,10 +938,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C15">
         <v>9</v>
@@ -931,10 +952,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -945,492 +966,562 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19">
         <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C20">
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21">
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C22">
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23">
         <v>17</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24">
         <v>18</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25">
         <v>19</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C26">
         <v>20</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C27">
         <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C31">
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C33">
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C34">
         <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C35">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C36">
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C37">
         <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C38">
         <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C39">
         <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>21</v>
-      </c>
-      <c r="B43" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43">
-        <v>3</v>
-      </c>
-      <c r="D43" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C44">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C45">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C46">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C47">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>46</v>
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C51">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>21</v>
-      </c>
-      <c r="B52" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52">
-        <v>4</v>
-      </c>
-      <c r="D52" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C53">
-        <v>5</v>
-      </c>
-      <c r="D53" t="s">
-        <v>86</v>
+        <v>1</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C54">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D54" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" t="s">
+        <v>67</v>
+      </c>
+      <c r="C59">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1441,10 +1532,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1304A835-0D3E-4B88-AD48-422BED80CB50}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A15"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1462,10 +1553,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1476,10 +1567,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1490,38 +1581,38 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1532,128 +1623,142 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
-        <v>30</v>
+      <c r="D9" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
         <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
         <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1663,10 +1768,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082625DD-20E7-4C98-A8A8-6BA57ED18482}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1684,10 +1789,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1698,24 +1803,24 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1726,66 +1831,66 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1796,69 +1901,69 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>82</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
         <v>80</v>
@@ -1866,72 +1971,86 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22">
         <v>7</v>
       </c>
-      <c r="D21" t="s">
-        <v>37</v>
+      <c r="D22" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed path finding, Marked old requirements, reworked interface
- Marked old requirements which we can discuss. These requirements are old and not yet implemented or implemented in another way.
- Moved some interface elements to make it more tidy
- Removed path finding
</commit_message>
<xml_diff>
--- a/conceptualisation/Requirements.xlsx
+++ b/conceptualisation/Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\Github\SEN1211-earthquake-project\conceptualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702DE86A-B2C7-4CBC-8C4E-BE926FE07B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91CA373-CE90-4D4E-92BA-51713518945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{574AE5E0-4647-4F58-AFB1-1899A91ECA14}"/>
+    <workbookView xWindow="-13896" yWindow="10116" windowWidth="23040" windowHeight="12204" xr2:uid="{574AE5E0-4647-4F58-AFB1-1899A91ECA14}"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="102">
   <si>
     <t>Drone flying time is affected by movement and hovering</t>
   </si>
@@ -130,9 +130,6 @@
     <t>Once ambulances face an closed road, they will try to find another route based on current knowledge.</t>
   </si>
   <si>
-    <t>Ambulance will check whether an road is open or closed at the start of the tick and drive through them during the tick.</t>
-  </si>
-  <si>
     <t>Roads will not be repaired.</t>
   </si>
   <si>
@@ -143,31 +140,6 @@
   </si>
   <si>
     <t>The simulation will run for 1-3 days (later aanpassen)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">During a trip, ambulances will check every </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ticks whether their current route is still valid, based on the information in the central system. </t>
-    </r>
   </si>
   <si>
     <t>The control room sends ambulances with patientience</t>
@@ -379,12 +351,18 @@
   <si>
     <t>Hospitals randomly hatched over crossings with at least 3 link-neighbors (connected to &gt;= roads)</t>
   </si>
+  <si>
+    <t>Ambulance will check whether a road is open or closed at the start of the tick and drive through them during the tick.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">During a trip, ambulances will check every N ticks whether their current route is still valid, based on the information in the central system. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +390,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -433,11 +418,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -744,7 +730,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,15 +738,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA006879-D9B2-4595-ABCF-2B2B08F25C3A}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>5</v>
       </c>
@@ -768,7 +754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -782,7 +768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -796,7 +782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -810,7 +796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -821,141 +807,142 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="4">
         <v>5</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12">
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="4">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="4">
         <v>7</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C15">
         <v>9</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -969,13 +956,13 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -983,13 +970,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -997,13 +984,13 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19">
         <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1011,13 +998,13 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C20">
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1025,13 +1012,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21">
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1039,13 +1026,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C22">
         <v>16</v>
       </c>
-      <c r="D22" t="s">
-        <v>76</v>
+      <c r="D22" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1053,13 +1040,13 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23">
         <v>17</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1067,13 +1054,13 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C24">
         <v>18</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1081,13 +1068,13 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C25">
         <v>19</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1095,13 +1082,13 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C26">
         <v>20</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1109,97 +1096,51 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27">
         <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28">
+        <v>22</v>
+      </c>
+      <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>16</v>
-      </c>
+      <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30" t="s">
-        <v>18</v>
-      </c>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31">
-        <v>3</v>
-      </c>
-      <c r="D31" t="s">
-        <v>17</v>
-      </c>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>50</v>
-      </c>
+      <c r="D32" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C34">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1207,13 +1148,13 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C35">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>98</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1221,13 +1162,13 @@
         <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C36">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1235,13 +1176,13 @@
         <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C37">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1249,13 +1190,13 @@
         <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C38">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1263,13 +1204,13 @@
         <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C39">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1277,13 +1218,13 @@
         <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C40">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1291,13 +1232,13 @@
         <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C41">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1305,13 +1246,27 @@
         <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C42">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" t="s">
         <v>52</v>
+      </c>
+      <c r="C43">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1319,13 +1274,13 @@
         <v>20</v>
       </c>
       <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44">
+        <v>11</v>
+      </c>
+      <c r="D44" t="s">
         <v>55</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1333,13 +1288,13 @@
         <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C45">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D45" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1347,13 +1302,13 @@
         <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1361,27 +1316,13 @@
         <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C47">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" t="s">
-        <v>55</v>
-      </c>
-      <c r="C48">
-        <v>5</v>
-      </c>
-      <c r="D48" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1389,13 +1330,13 @@
         <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C49">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1403,13 +1344,13 @@
         <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C50">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1417,13 +1358,27 @@
         <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C51">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1431,13 +1386,13 @@
         <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>45</v>
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1445,13 +1400,13 @@
         <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D54" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1459,13 +1414,13 @@
         <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C55">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1473,27 +1428,13 @@
         <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C56">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>20</v>
-      </c>
-      <c r="B57" t="s">
-        <v>67</v>
-      </c>
-      <c r="C57">
-        <v>5</v>
-      </c>
-      <c r="D57" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1501,13 +1442,13 @@
         <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C58">
-        <v>7</v>
-      </c>
-      <c r="D58" t="s">
-        <v>96</v>
+        <v>1</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1515,13 +1456,83 @@
         <v>20</v>
       </c>
       <c r="B59" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>5</v>
+      </c>
+      <c r="D62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64">
         <v>8</v>
       </c>
-      <c r="D59" t="s">
-        <v>101</v>
+      <c r="D64" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1535,7 +1546,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1590,7 +1601,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1604,7 +1615,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1617,7 +1628,7 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1646,7 +1657,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1660,7 +1671,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1687,8 +1698,8 @@
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" t="s">
-        <v>64</v>
+      <c r="D11" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1702,7 +1713,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1716,7 +1727,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1729,8 +1740,8 @@
       <c r="C14">
         <v>13</v>
       </c>
-      <c r="D14" t="s">
-        <v>35</v>
+      <c r="D14" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1743,8 +1754,8 @@
       <c r="C15">
         <v>14</v>
       </c>
-      <c r="D15" t="s">
-        <v>44</v>
+      <c r="D15" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1758,11 +1769,12 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1771,7 +1783,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1792,7 +1804,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1806,13 +1818,13 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1820,7 +1832,7 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1834,13 +1846,13 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1848,13 +1860,13 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1862,13 +1874,13 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1876,13 +1888,13 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1890,7 +1902,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1904,13 +1916,13 @@
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1918,13 +1930,13 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1932,13 +1944,13 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1946,13 +1958,13 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1960,13 +1972,13 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
-        <v>80</v>
+      <c r="D16" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1974,13 +1986,13 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
-        <v>78</v>
+      <c r="D17" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1988,13 +2000,13 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
-      <c r="D18" t="s">
-        <v>79</v>
+      <c r="D18" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2002,13 +2014,13 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2016,13 +2028,13 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2030,13 +2042,13 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2044,13 +2056,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22">
         <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Marked some old requirements
These requirements are old and are either not implemented or implemented in another way. They will be deleted or rephrased.
</commit_message>
<xml_diff>
--- a/conceptualisation/Requirements.xlsx
+++ b/conceptualisation/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\Github\SEN1211-earthquake-project\conceptualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91CA373-CE90-4D4E-92BA-51713518945E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BB29D7-B1E6-4DC7-AFA5-B685C10AC4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13896" yWindow="10116" windowWidth="23040" windowHeight="12204" xr2:uid="{574AE5E0-4647-4F58-AFB1-1899A91ECA14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{574AE5E0-4647-4F58-AFB1-1899A91ECA14}"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -362,7 +362,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,6 +397,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -418,12 +432,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -740,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA006879-D9B2-4595-ABCF-2B2B08F25C3A}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -876,7 +892,7 @@
       <c r="C11" s="4">
         <v>5</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="4"/>
@@ -891,7 +907,7 @@
       <c r="C12" s="4">
         <v>6</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -905,7 +921,7 @@
       <c r="C13" s="4">
         <v>7</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -919,7 +935,7 @@
       <c r="C14">
         <v>8</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -933,7 +949,7 @@
       <c r="C15">
         <v>9</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -947,7 +963,7 @@
       <c r="C16">
         <v>10</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -961,7 +977,7 @@
       <c r="C17">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="5" t="s">
         <v>59</v>
       </c>
     </row>
@@ -975,7 +991,7 @@
       <c r="C18">
         <v>12</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -989,7 +1005,7 @@
       <c r="C19">
         <v>13</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1003,7 +1019,7 @@
       <c r="C20">
         <v>14</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="5" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1017,7 +1033,7 @@
       <c r="C21">
         <v>15</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1031,7 +1047,7 @@
       <c r="C22">
         <v>16</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="5" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1045,7 +1061,7 @@
       <c r="C23">
         <v>17</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1059,7 +1075,7 @@
       <c r="C24">
         <v>18</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1073,7 +1089,7 @@
       <c r="C25">
         <v>19</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1087,7 +1103,7 @@
       <c r="C26">
         <v>20</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1628,7 +1644,7 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1740,7 +1756,7 @@
       <c r="C14">
         <v>13</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="6" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1754,7 +1770,7 @@
       <c r="C15">
         <v>14</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1782,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082625DD-20E7-4C98-A8A8-6BA57ED18482}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1977,7 +1993,7 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1991,7 +2007,7 @@
       <c r="C17">
         <v>2</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="5" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2005,7 +2021,7 @@
       <c r="C18">
         <v>3</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated requirements, images to folder
-Updated the requirements slightly
- Put all the images for the conceptualisation chapter into a folder
</commit_message>
<xml_diff>
--- a/conceptualisation/Requirements.xlsx
+++ b/conceptualisation/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\Github\SEN1211-earthquake-project\conceptualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DF35A1-9DF8-4A3A-A55B-DA452F92DDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971FBBC7-B45D-434F-8AAA-146DBBAF7C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3456" yWindow="3456" windowWidth="23040" windowHeight="12204" xr2:uid="{574AE5E0-4647-4F58-AFB1-1899A91ECA14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{574AE5E0-4647-4F58-AFB1-1899A91ECA14}"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>Drones have a 360 degree view with certain range</t>
   </si>
   <si>
-    <t>Hospitals, buildings, roads, crossings,  residents and drones are objects</t>
-  </si>
-  <si>
     <t>Requirement</t>
   </si>
   <si>
@@ -377,6 +374,9 @@
   </si>
   <si>
     <t>If the hospital is full when the ambulances arrives, it will select and drive to another hospital</t>
+  </si>
+  <si>
+    <t>Hospitals, buildings, roads, crossings,  residents  are objects</t>
   </si>
 </sst>
 </file>
@@ -737,648 +737,651 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA006879-D9B2-4595-ABCF-2B2B08F25C3A}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1">
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1">
         <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1">
         <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1">
         <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1">
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1">
         <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1">
         <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1">
         <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1">
         <v>29</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1">
         <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1">
         <v>31</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1">
         <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25">
         <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26">
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28">
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29">
         <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30">
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31">
         <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32">
         <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36">
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38">
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C40">
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45">
         <v>3</v>
       </c>
       <c r="D45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C46">
         <v>4</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C47">
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C48">
         <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C49">
         <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1395,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1402,326 +1405,326 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18">
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19">
         <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20">
         <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21">
         <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22">
         <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23">
         <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
         <v>11</v>
-      </c>
-      <c r="B25" t="s">
-        <v>12</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1732,10 +1735,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
         <v>11</v>
-      </c>
-      <c r="B26" t="s">
-        <v>12</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -1746,184 +1749,184 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
         <v>11</v>
-      </c>
-      <c r="B27" t="s">
-        <v>12</v>
       </c>
       <c r="C27">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
         <v>11</v>
-      </c>
-      <c r="B28" t="s">
-        <v>12</v>
       </c>
       <c r="C28">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
         <v>11</v>
-      </c>
-      <c r="B29" t="s">
-        <v>12</v>
       </c>
       <c r="C29">
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
         <v>11</v>
-      </c>
-      <c r="B30" t="s">
-        <v>12</v>
       </c>
       <c r="C30">
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
         <v>11</v>
-      </c>
-      <c r="B31" t="s">
-        <v>12</v>
       </c>
       <c r="C31">
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
         <v>11</v>
       </c>
-      <c r="B32" t="s">
-        <v>12</v>
-      </c>
       <c r="C32">
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
         <v>11</v>
-      </c>
-      <c r="B33" t="s">
-        <v>12</v>
       </c>
       <c r="C33">
         <v>11</v>
       </c>
       <c r="D33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
         <v>11</v>
       </c>
-      <c r="B34" t="s">
-        <v>12</v>
-      </c>
       <c r="C34">
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
         <v>11</v>
       </c>
-      <c r="B35" t="s">
-        <v>12</v>
-      </c>
       <c r="C35">
         <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
         <v>11</v>
-      </c>
-      <c r="B36" t="s">
-        <v>12</v>
       </c>
       <c r="C36">
         <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
         <v>11</v>
-      </c>
-      <c r="B37" t="s">
-        <v>12</v>
       </c>
       <c r="C37">
         <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
         <v>11</v>
-      </c>
-      <c r="B38" t="s">
-        <v>12</v>
       </c>
       <c r="C38">
         <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
         <v>11</v>
-      </c>
-      <c r="B39" t="s">
-        <v>12</v>
       </c>
       <c r="C39">
         <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1936,8 +1939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082625DD-20E7-4C98-A8A8-6BA57ED18482}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1947,248 +1950,248 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated requirements, Added folder final submission
- Updated some requirements according to what is modelled
- Added a folder for the final submission file
</commit_message>
<xml_diff>
--- a/conceptualisation/Requirements.xlsx
+++ b/conceptualisation/Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\Github\SEN1211-earthquake-project\conceptualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971FBBC7-B45D-434F-8AAA-146DBBAF7C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E0A5A2-5080-4E81-B4F7-997DA6792413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{574AE5E0-4647-4F58-AFB1-1899A91ECA14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{574AE5E0-4647-4F58-AFB1-1899A91ECA14}"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="117">
   <si>
     <t>Drone flying time is affected by movement and hovering</t>
   </si>
@@ -148,12 +148,6 @@
     <t>MN</t>
   </si>
   <si>
-    <t>Tall buildings have between 11 and 20 residents.</t>
-  </si>
-  <si>
-    <t>Medium sized building have between 6 and 10 residents.</t>
-  </si>
-  <si>
     <t>Small building have between 1 and 5 residents.</t>
   </si>
   <si>
@@ -377,13 +371,31 @@
   </si>
   <si>
     <t>Hospitals, buildings, roads, crossings,  residents  are objects</t>
+  </si>
+  <si>
+    <t>10% Of buildings are tall, 30% medium-height and 60% small</t>
+  </si>
+  <si>
+    <t>Medium sized building have between 5 and 10 residents.</t>
+  </si>
+  <si>
+    <t>Tall buildings have between 10 and 20 residents.</t>
+  </si>
+  <si>
+    <t>The health of residents in a collapsed building are initialized according to normal distribution with average 0.8 and standard deviation 0.3</t>
+  </si>
+  <si>
+    <t>The health of residents in a high-damage building are initialized according to normal distribution with average 0.95 and standard deviation 0.3</t>
+  </si>
+  <si>
+    <t>Drones start with a 100% full battery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,6 +405,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -735,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA006879-D9B2-4595-ABCF-2B2B08F25C3A}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -793,7 +811,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -821,7 +839,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -835,7 +853,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -849,7 +867,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -863,7 +881,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -877,7 +895,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -891,7 +909,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -905,7 +923,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -919,7 +937,7 @@
         <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -933,7 +951,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -947,7 +965,7 @@
         <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -961,7 +979,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -975,35 +993,35 @@
         <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1">
+        <v>33</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1">
+        <v>34</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1014,10 +1032,10 @@
         <v>33</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1028,10 +1046,10 @@
         <v>33</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1042,10 +1060,10 @@
         <v>33</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1056,10 +1074,10 @@
         <v>33</v>
       </c>
       <c r="C24">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1070,10 +1088,10 @@
         <v>33</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1084,10 +1102,10 @@
         <v>33</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1098,10 +1116,10 @@
         <v>33</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1112,10 +1130,10 @@
         <v>33</v>
       </c>
       <c r="C28">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1126,10 +1144,10 @@
         <v>33</v>
       </c>
       <c r="C29">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1140,10 +1158,10 @@
         <v>33</v>
       </c>
       <c r="C30">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1154,10 +1172,10 @@
         <v>33</v>
       </c>
       <c r="C31">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D31" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1168,10 +1186,24 @@
         <v>33</v>
       </c>
       <c r="C32">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1179,13 +1211,13 @@
         <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1193,27 +1225,13 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36">
-        <v>3</v>
-      </c>
-      <c r="D36" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1224,10 +1242,10 @@
         <v>34</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1238,10 +1256,10 @@
         <v>34</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1252,10 +1270,10 @@
         <v>34</v>
       </c>
       <c r="C39">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1266,10 +1284,10 @@
         <v>34</v>
       </c>
       <c r="C40">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1280,10 +1298,24 @@
         <v>34</v>
       </c>
       <c r="C41">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>19</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1291,13 +1323,13 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1305,27 +1337,13 @@
         <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>10</v>
-      </c>
-      <c r="B45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45">
-        <v>3</v>
-      </c>
-      <c r="D45" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1333,13 +1351,13 @@
         <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C46">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1347,10 +1365,10 @@
         <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D47" t="s">
         <v>47</v>
@@ -1361,13 +1379,13 @@
         <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C48">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1375,16 +1393,59 @@
         <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52">
         <v>8</v>
       </c>
-      <c r="D49" t="s">
-        <v>62</v>
+      <c r="D52" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1392,10 +1453,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1304A835-0D3E-4B88-AD48-422BED80CB50}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1436,7 +1497,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1478,7 +1539,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1492,7 +1553,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1506,7 +1567,7 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1534,7 +1595,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1562,7 +1623,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1576,7 +1637,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1590,7 +1651,7 @@
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1604,7 +1665,7 @@
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1618,7 +1679,7 @@
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1632,7 +1693,7 @@
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1646,7 +1707,7 @@
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1660,7 +1721,7 @@
         <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1674,7 +1735,7 @@
         <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1688,7 +1749,7 @@
         <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1702,7 +1763,7 @@
         <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1716,7 +1777,7 @@
         <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1758,7 +1819,7 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1772,7 +1833,7 @@
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1786,7 +1847,7 @@
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1800,7 +1861,7 @@
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1814,7 +1875,7 @@
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1828,7 +1889,7 @@
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1842,7 +1903,7 @@
         <v>11</v>
       </c>
       <c r="D33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1856,7 +1917,7 @@
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1870,7 +1931,7 @@
         <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1884,7 +1945,7 @@
         <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1898,7 +1959,7 @@
         <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1912,7 +1973,7 @@
         <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1926,7 +1987,21 @@
         <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>18</v>
+      </c>
+      <c r="D40" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1939,7 +2014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082625DD-20E7-4C98-A8A8-6BA57ED18482}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -1995,7 +2070,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2009,7 +2084,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2023,7 +2098,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2037,7 +2112,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2051,7 +2126,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2065,7 +2140,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -2073,7 +2148,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2087,13 +2162,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2101,13 +2176,13 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -2115,7 +2190,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -2129,13 +2204,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2143,13 +2218,13 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2157,13 +2232,13 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2171,13 +2246,13 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2185,13 +2260,13 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated requirements and req images
- Updated some requirements for residents (healh increase and degradation based on medical-treatment) and drones (starting with full battery
- Updated the images that belong to the requirements
</commit_message>
<xml_diff>
--- a/conceptualisation/Requirements.xlsx
+++ b/conceptualisation/Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\Github\SEN1211-earthquake-project\conceptualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E0A5A2-5080-4E81-B4F7-997DA6792413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCC3F8E-50F4-4296-8697-315A6104795C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{574AE5E0-4647-4F58-AFB1-1899A91ECA14}"/>
   </bookViews>
@@ -436,9 +436,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -755,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA006879-D9B2-4595-ABCF-2B2B08F25C3A}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1453,15 +1454,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1304A835-0D3E-4B88-AD48-422BED80CB50}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -2015,7 +2017,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>